<commit_message>
changes for upto manuscript v3
</commit_message>
<xml_diff>
--- a/GAM_models/Summary_results/summary_all_buildings.xlsx
+++ b/GAM_models/Summary_results/summary_all_buildings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laxmandahal/Desktop/UCLA/Phd/Research/IM_study/Codes/GAM_models/Summary_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D88263-3304-684E-9D76-D3FB0686845D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC764758-37B6-D744-A7E0-4C4597BC9FFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-31720" yWindow="-380" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>SaT1</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t xml:space="preserve">none </t>
+  </si>
+  <si>
+    <t>Percent Sufficiency- MVN GAM Model</t>
   </si>
 </sst>
 </file>
@@ -592,7 +595,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -610,6 +613,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -967,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -979,124 +985,120 @@
     <col min="2" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H3" s="4">
         <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="4">
-        <v>38</v>
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4">
-        <v>25</v>
-      </c>
-      <c r="I5" s="1">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4">
+        <v>25</v>
+      </c>
+      <c r="I6" s="1">
         <v>13</v>
-      </c>
-      <c r="C6" s="4">
-        <v>38</v>
-      </c>
-      <c r="H6" s="6">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="4">
-        <v>56</v>
-      </c>
-      <c r="E7" s="1">
-        <v>19</v>
-      </c>
-      <c r="H7" s="1">
-        <v>31</v>
+        <v>38</v>
+      </c>
+      <c r="H7" s="6">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1">
+        <v>14</v>
+      </c>
+      <c r="C8" s="4">
+        <v>56</v>
+      </c>
+      <c r="E8" s="1">
         <v>19</v>
       </c>
-      <c r="C8" s="4">
+      <c r="H8" s="1">
         <v>31</v>
-      </c>
-      <c r="E8" s="1">
-        <v>25</v>
-      </c>
-      <c r="H8" s="1">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1">
         <v>19</v>
       </c>
       <c r="C9" s="4">
-        <v>38</v>
-      </c>
-      <c r="E9" s="6">
-        <v>38</v>
+        <v>31</v>
+      </c>
+      <c r="E9" s="1">
+        <v>25</v>
       </c>
       <c r="H9" s="1">
         <v>25</v>
@@ -1104,57 +1106,78 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1">
-        <v>28</v>
-      </c>
-      <c r="D10" s="4">
-        <v>44</v>
-      </c>
-      <c r="E10" s="1">
-        <v>41</v>
-      </c>
-      <c r="F10" s="1">
-        <v>6</v>
-      </c>
-      <c r="G10" s="1">
-        <v>41</v>
+        <v>19</v>
+      </c>
+      <c r="C10" s="4">
+        <v>38</v>
+      </c>
+      <c r="E10" s="6">
+        <v>38</v>
       </c>
       <c r="H10" s="1">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1">
         <v>6</v>
       </c>
       <c r="C11" s="1">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D11" s="4">
         <v>44</v>
       </c>
       <c r="E11" s="1">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F11" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G11" s="1">
         <v>41</v>
       </c>
       <c r="H11" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1">
+        <v>25</v>
+      </c>
+      <c r="D12" s="4">
+        <v>44</v>
+      </c>
+      <c r="E12" s="1">
+        <v>28</v>
+      </c>
+      <c r="F12" s="1">
+        <v>9</v>
+      </c>
+      <c r="G12" s="1">
+        <v>41</v>
+      </c>
+      <c r="H12" s="1">
         <v>19</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:I1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>